<commit_message>
CDS Library source query fixed
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_CDS_Filter_LibrarySource_BulkWholeCell.xlsx
+++ b/InputFiles/TC01_CDS_Filter_LibrarySource_BulkWholeCell.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0620\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0717new\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127879D3-A337-4020-B87C-3FC2E7407C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F09AB6A-7393-4E3C-AF0F-99D6C176543B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -104,19 +104,24 @@
    LIMIT 100</t>
   </si>
   <si>
-    <t>MATCH (f:file)
-MATCH (g:genomic_info)
-WHERE g.library_source in ['Bulk Whole Cell']
-MATCH (g)--&gt;(f:file)--&gt;(samp:sample)--&gt;(p:participant)--&gt;(s:study)
-MATCH (samp:sample)--&gt;(p)
-WITH p, s, collect(samp.sample_id) as samp
+    <t>MATCH (p:participant)--&gt;(s:study)
+OPTIONAL MATCH (samp:sample)--&gt;(p)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+OPTIONAL MATCH (f)&lt;--(g:genomic_info)
+WITH s, p, samp, f, g, diag
+WHERE g.library_source in['Bulk Whole Cell']
+WITH p
+OPTIONAL MATCH (p)--&gt;(s:study)
+OPTIONAL MATCH (samp:sample)--&gt;(p)
+WITH s, p, apoc.coll.sort(collect(distinct samp.sample_id)) as samp
 RETURN 
-    coalesce(p.participant_id,'') as `Participant ID`,
-    coalesce(s.study_name, '') as `Study Name`,
-    coalesce(s.phs_accession,'') as `Accession`,
-    coalesce(p.gender,'') as `Gender`,
-    coalesce(apoc.text.join(samp, ','), '') as `Samples`
-ORDER BY `Participant ID`
+coalesce(p.participant_id,'') as `Participant ID`,
+coalesce(s.study_name, '') as `Study Name`,
+coalesce(s.phs_accession,'') as `Accession`,
+coalesce(p.gender,'') as `Gender`,
+coalesce(apoc.text.join(samp, ','), '') as `Samples`
+ORDER BY p.participant_id
 LIMIT 100</t>
   </si>
 </sst>
@@ -146,7 +151,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="15"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -176,9 +181,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -500,36 +503,37 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.7109375" customWidth="1"/>
-    <col min="4" max="4" width="70.28515625" customWidth="1"/>
-    <col min="5" max="5" width="63.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="63.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="220.5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="390" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -538,15 +542,15 @@
       <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="204.75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" ht="292.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -555,15 +559,15 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="220.5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="292.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -572,19 +576,19 @@
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>